<commit_message>
Add benchmarks for Core i7 6820HK (mainstream Skylake).
</commit_message>
<xml_diff>
--- a/Benchmarks/Benchmarks.xlsx
+++ b/Benchmarks/Benchmarks.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="12435" windowHeight="10035" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="12435" windowHeight="10035" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="FX-8350" sheetId="1" r:id="rId1"/>
     <sheet name="i7 3630QM" sheetId="3" r:id="rId2"/>
     <sheet name="i7 4770k" sheetId="2" r:id="rId3"/>
+    <sheet name="i7 6820HK" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="22">
   <si>
     <t>AMD FX-8350</t>
   </si>
@@ -80,6 +81,9 @@
   <si>
     <t>Intel Core i7 3630QM</t>
   </si>
+  <si>
+    <t>Intel Core i7 6820HK</t>
+  </si>
 </sst>
 </file>
 
@@ -130,74 +134,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -214,7 +150,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFECF5"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1066,7 +1002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -1423,7 +1359,7 @@
   <dimension ref="B2:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H22"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1872,4 +1808,463 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:H22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>3.2046700000000001</v>
+      </c>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>32</v>
+      </c>
+      <c r="F4" s="1">
+        <f>E$2*E4</f>
+        <v>102.54944</v>
+      </c>
+      <c r="G4" s="1">
+        <v>101.39100000000001</v>
+      </c>
+      <c r="H4" s="2">
+        <f>G4/F4</f>
+        <v>0.98870359506595062</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>32</v>
+      </c>
+      <c r="F5" s="1">
+        <f>E$2*E5</f>
+        <v>102.54944</v>
+      </c>
+      <c r="G5" s="1">
+        <v>100.002</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" ref="H5:H7" si="0">G5/F5</f>
+        <v>0.97515890871759014</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>32</v>
+      </c>
+      <c r="F6" s="1">
+        <f>E$2*E6</f>
+        <v>102.54944</v>
+      </c>
+      <c r="G6" s="1">
+        <v>100.322</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.97827935481656458</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>64</v>
+      </c>
+      <c r="F7" s="1">
+        <f>E$2*E7</f>
+        <v>205.09888000000001</v>
+      </c>
+      <c r="G7" s="1">
+        <v>204.45</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99683625771140227</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>16</v>
+      </c>
+      <c r="F9" s="1">
+        <f>E$2*E9</f>
+        <v>51.274720000000002</v>
+      </c>
+      <c r="G9" s="1">
+        <v>50.891100000000002</v>
+      </c>
+      <c r="H9" s="2">
+        <f>G9/F9</f>
+        <v>0.99251834042194675</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>16</v>
+      </c>
+      <c r="F10" s="1">
+        <f>E$2*E10</f>
+        <v>51.274720000000002</v>
+      </c>
+      <c r="G10" s="1">
+        <v>50.101399999999998</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" ref="H10:H12" si="1">G10/F10</f>
+        <v>0.97711698864469654</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>16</v>
+      </c>
+      <c r="F11" s="1">
+        <f>E$2*E11</f>
+        <v>51.274720000000002</v>
+      </c>
+      <c r="G11" s="1">
+        <v>50.167200000000001</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.97840027210289982</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>32</v>
+      </c>
+      <c r="F12" s="1">
+        <f>E$2*E12</f>
+        <v>102.54944</v>
+      </c>
+      <c r="G12" s="1">
+        <v>102.113</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="1"/>
+        <v>0.99574410157676141</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>64</v>
+      </c>
+      <c r="F14" s="1">
+        <f>E$2*E14</f>
+        <v>205.09888000000001</v>
+      </c>
+      <c r="G14">
+        <v>200.589</v>
+      </c>
+      <c r="H14" s="2">
+        <f>G14/F14</f>
+        <v>0.97801119147993387</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <v>64</v>
+      </c>
+      <c r="F15" s="1">
+        <f>E$2*E15</f>
+        <v>205.09888000000001</v>
+      </c>
+      <c r="G15">
+        <v>199.18700000000001</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" ref="H15:H17" si="2">G15/F15</f>
+        <v>0.9711754642443684</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16">
+        <v>64</v>
+      </c>
+      <c r="F16" s="1">
+        <f>E$2*E16</f>
+        <v>205.09888000000001</v>
+      </c>
+      <c r="G16">
+        <v>199.86</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="2"/>
+        <v>0.97445680834532111</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>128</v>
+      </c>
+      <c r="F17" s="1">
+        <f>E$2*E17</f>
+        <v>410.19776000000002</v>
+      </c>
+      <c r="G17">
+        <v>408.24799999999999</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="2"/>
+        <v>0.99524678047973736</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>32</v>
+      </c>
+      <c r="F19" s="1">
+        <f>E$2*E19</f>
+        <v>102.54944</v>
+      </c>
+      <c r="G19">
+        <v>100.42400000000001</v>
+      </c>
+      <c r="H19" s="2">
+        <f>G19/F19</f>
+        <v>0.97927399701061268</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>32</v>
+      </c>
+      <c r="F20" s="1">
+        <f>E$2*E20</f>
+        <v>102.54944</v>
+      </c>
+      <c r="G20">
+        <v>98.087000000000003</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" ref="H20:H22" si="3">G20/F20</f>
+        <v>0.95648498909404089</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21">
+        <v>32</v>
+      </c>
+      <c r="F21" s="1">
+        <f>E$2*E21</f>
+        <v>102.54944</v>
+      </c>
+      <c r="G21">
+        <v>99.905199999999994</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" si="3"/>
+        <v>0.97421497377265043</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22">
+        <v>64</v>
+      </c>
+      <c r="F22" s="1">
+        <f>E$2*E22</f>
+        <v>205.09888000000001</v>
+      </c>
+      <c r="G22">
+        <v>204.166</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" si="3"/>
+        <v>0.99545155975498256</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>